<commit_message>
clean respository and rebuild the parser of database
</commit_message>
<xml_diff>
--- a/benchmark-PLDI26/efficiency/testData.xlsx
+++ b/benchmark-PLDI26/efficiency/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizi/Desktop/pl/getprime/benchmark-PLDI26/efficiency/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF48B151-399C-8040-A269-E6D59E8A20C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1F4DCE-8722-5146-8217-5007CB03E9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="15520" xr2:uid="{1056904E-6764-8A46-AF04-B89D31D65114}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:Y6"/>
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>